<commit_message>
Remove year 2018 data as it is not yet complete
</commit_message>
<xml_diff>
--- a/docs/Data/CitationsYear.xlsx
+++ b/docs/Data/CitationsYear.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lrutter/Desktop/PubCode/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lrutter/Desktop/PubCode/docs/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1480" yWindow="460" windowWidth="24360" windowHeight="14820" tabRatio="500"/>
+    <workbookView xWindow="1240" yWindow="460" windowWidth="24360" windowHeight="14820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -486,7 +486,7 @@
   <dimension ref="A1:K1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>